<commit_message>
Studija izvedivosti - dodani komentari
</commit_message>
<xml_diff>
--- a/docs/NeighbourConnect-StudijaIzvedivosti.xlsx
+++ b/docs/NeighbourConnect-StudijaIzvedivosti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\Private\FER\Semestar8\Kolegiji\infsus\projekt\NeighbourConnect\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4F4F22-3017-4314-A579-915303075955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D91E4B-D4AB-45BF-A7A5-EB5963AF694A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StudijaIzvedivosti" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Karakteristike</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>Plaće 2*1100/mj</t>
+  </si>
+  <si>
+    <t>Vlastita izrada pruža najfleksibilniju izvedivost projekta. Nedostatak je što zahtjeva najviše vremena (modeliranje i izgradnja baze podataka, izrada korisničkog sučelja). Prednost je manji ekonomski trošak i općenita fleksibilnost u tehnološkim aspektima. Imat ćemo točnu i potrebnu količinu funkcionalnosti koje su nam potrebne za uspješno ostvarivanje projekta.</t>
+  </si>
+  <si>
+    <t>Nadogradnja sustava može biti tehnički i operativno izazovan proces zbog korištenih tehnologija kojima se moramo prilagoditi. U pravilu je vremenski povoljnije od vlastite izrade s obzirom da određene funkcionalnosti već postoje u sustavu.</t>
+  </si>
+  <si>
+    <t>Vremenski najpovoljnije rješenje jer kupujemo gotov proizvod. Međutim, ekonomski je vrlo nepovoljno rješenje s obzirom da plaćamo niz usluga. Također, dobiveno rješenje može sadržavati puno više funkcionalnosti nego što je potrebno za normalan rad našeg sustava.</t>
   </si>
 </sst>
 </file>
@@ -220,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -778,6 +787,15 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -823,7 +841,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1060,7 +1078,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1068,21 +1086,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1389,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EEE08C-145C-49B9-A7B2-D920AF3FF34A}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,7 +1430,7 @@
     <col min="1" max="10" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="52" t="s">
         <v>15</v>
       </c>
@@ -1430,7 +1460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="64" t="s">
         <v>2</v>
       </c>
@@ -1461,9 +1491,19 @@
       <c r="J2" s="3">
         <v>3</v>
       </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K2" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
       <c r="B3" s="62" t="s">
         <v>18</v>
@@ -1492,9 +1532,17 @@
       <c r="J3" s="4">
         <v>3</v>
       </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K3" s="103"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
       <c r="B4" s="62" t="s">
         <v>19</v>
@@ -1523,9 +1571,17 @@
       <c r="J4" s="4">
         <v>2</v>
       </c>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="103"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104"/>
+      <c r="N4" s="104"/>
+      <c r="O4" s="104"/>
+      <c r="P4" s="104"/>
+      <c r="Q4" s="104"/>
+      <c r="R4" s="104"/>
+      <c r="S4" s="104"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="66"/>
       <c r="B5" s="63" t="s">
         <v>20</v>
@@ -1554,9 +1610,17 @@
       <c r="J5" s="10">
         <v>3</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="103"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>21</v>
       </c>
@@ -1595,7 +1659,7 @@
       </c>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="64" t="s">
         <v>16</v>
       </c>
@@ -1626,9 +1690,19 @@
       <c r="J7" s="13">
         <v>1</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K7" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="106"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="106"/>
+      <c r="Q7" s="106"/>
+      <c r="R7" s="106"/>
+      <c r="S7" s="106"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
       <c r="B8" s="62" t="s">
         <v>18</v>
@@ -1657,9 +1731,17 @@
       <c r="J8" s="4">
         <v>2</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K8" s="105"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="106"/>
+      <c r="O8" s="106"/>
+      <c r="P8" s="106"/>
+      <c r="Q8" s="106"/>
+      <c r="R8" s="106"/>
+      <c r="S8" s="106"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="65"/>
       <c r="B9" s="62" t="s">
         <v>19</v>
@@ -1688,9 +1770,17 @@
       <c r="J9" s="4">
         <v>2</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="105"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="106"/>
+      <c r="N9" s="106"/>
+      <c r="O9" s="106"/>
+      <c r="P9" s="106"/>
+      <c r="Q9" s="106"/>
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="66"/>
       <c r="B10" s="63" t="s">
         <v>20</v>
@@ -1719,8 +1809,17 @@
       <c r="J10" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="105"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="106"/>
+      <c r="N10" s="106"/>
+      <c r="O10" s="106"/>
+      <c r="P10" s="106"/>
+      <c r="Q10" s="106"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="106"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1857,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="64" t="s">
         <v>3</v>
       </c>
@@ -1789,8 +1888,19 @@
       <c r="J12" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="105" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="106"/>
+      <c r="M12" s="106"/>
+      <c r="N12" s="106"/>
+      <c r="O12" s="106"/>
+      <c r="P12" s="106"/>
+      <c r="Q12" s="106"/>
+      <c r="R12" s="106"/>
+      <c r="S12" s="106"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="65"/>
       <c r="B13" s="62" t="s">
         <v>18</v>
@@ -1819,8 +1929,17 @@
       <c r="J13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K13" s="105"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="106"/>
+      <c r="S13" s="106"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="65"/>
       <c r="B14" s="62" t="s">
         <v>19</v>
@@ -1849,8 +1968,17 @@
       <c r="J14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K14" s="105"/>
+      <c r="L14" s="106"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="106"/>
+      <c r="O14" s="106"/>
+      <c r="P14" s="106"/>
+      <c r="Q14" s="106"/>
+      <c r="R14" s="106"/>
+      <c r="S14" s="106"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="66"/>
       <c r="B15" s="63" t="s">
         <v>20</v>
@@ -1879,8 +2007,17 @@
       <c r="J15" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K15" s="105"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="106"/>
+      <c r="N15" s="106"/>
+      <c r="O15" s="106"/>
+      <c r="P15" s="106"/>
+      <c r="Q15" s="106"/>
+      <c r="R15" s="106"/>
+      <c r="S15" s="106"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>21</v>
       </c>
@@ -1993,11 +2130,14 @@
       <c r="J20" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A17:J17"/>
+    <mergeCell ref="K2:S5"/>
+    <mergeCell ref="K7:S10"/>
+    <mergeCell ref="K12:S15"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:A5"/>
@@ -2012,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39DF403-A7BE-48D5-8475-75278B66FAF2}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2284,7 +2424,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>